<commit_message>
Form fixes for Sunday
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
+++ b/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -72,6 +72,9 @@
     <t xml:space="preserve">display.constraint_message</t>
   </si>
   <si>
+    <t xml:space="preserve">hideInContents</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin screen</t>
   </si>
   <si>
@@ -129,13 +132,31 @@
     <t xml:space="preserve">q65d</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q65e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not(selected(data('hh_death_date_dk'), 'dk'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth_date</t>
   </si>
   <si>
     <t xml:space="preserve">hh_death_date</t>
   </si>
   <si>
-    <t xml:space="preserve">q65e</t>
+    <t xml:space="preserve">selected(data('hh_death_date_dk'), 'dk') || !data('hh_death_date') || (!data('hh_death_date').isBefore('2020-03-01') &amp;&amp; !data('hh_death_date').isAfter())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid_death_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
   </si>
   <si>
     <t xml:space="preserve">select_multiple</t>
@@ -147,9 +168,6 @@
     <t xml:space="preserve">hh_death_date_dk</t>
   </si>
   <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
     <t xml:space="preserve">selected(data('hh_death_date_dk'), 'dk')</t>
   </si>
   <si>
@@ -159,9 +177,6 @@
     <t xml:space="preserve">null</t>
   </si>
   <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
     <t xml:space="preserve">integer</t>
   </si>
   <si>
@@ -355,6 +370,9 @@
   </si>
   <si>
     <t xml:space="preserve">ID must be in this format ABC-123-701 (3 capital letters, '-', 3 numbers, '-', 7##).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date cannot be in the future&lt;br&gt;Date should be in the past 12 months</t>
   </si>
 </sst>
 </file>
@@ -457,7 +475,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -497,13 +515,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.83"/>
@@ -516,6 +534,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,85 +575,85 @@
       <c r="L1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -641,60 +661,93 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
+      <c r="A8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="L9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="A10" s="0" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="0" t="n">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>48</v>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +772,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
@@ -728,46 +781,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -789,10 +842,10 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
@@ -808,58 +861,58 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -881,10 +934,10 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.47"/>
@@ -896,41 +949,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20210203001</v>
@@ -938,74 +991,74 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1024,85 +1077,86 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="38.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,93 +1164,101 @@
         <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>